<commit_message>
more demo data, period and scenario selectors depend on country availability
</commit_message>
<xml_diff>
--- a/data/JAM_ADM1_CF_2020.xlsx
+++ b/data/JAM_ADM1_CF_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\Documents\GitHub\CCDR-geoboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A6FB0E-E523-4980-A89F-680A16407BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B71303E-5E65-40AF-8D1C-ACA88951E1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="15310" windowHeight="13090" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="590" windowWidth="15310" windowHeight="13090" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POP_EAI_function" sheetId="1" r:id="rId1"/>
@@ -4222,7 +4222,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD13"/>
+      <selection activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>